<commit_message>
update first progress on imdb
</commit_message>
<xml_diff>
--- a/noise_defense_attack_result/paper_default setting/AGNEWS/results.xlsx
+++ b/noise_defense_attack_result/paper_default setting/AGNEWS/results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="155">
   <si>
     <t>Models</t>
   </si>
@@ -22,78 +22,372 @@
     <t>Clean Accuracy (%)</t>
   </si>
   <si>
+    <t>textbugger</t>
+  </si>
+  <si>
+    <t>AuA(%) (ASR(%)↓)</t>
+  </si>
+  <si>
+    <t>Avg. Query↓</t>
+  </si>
+  <si>
+    <t>BERT</t>
+  </si>
+  <si>
+    <t>35.20% (62.63%)</t>
+  </si>
+  <si>
+    <t>351.92</t>
+  </si>
+  <si>
+    <t>94.20%</t>
+  </si>
+  <si>
+    <t>BERT_ASCC</t>
+  </si>
+  <si>
+    <t>39.30% (55.94%)</t>
+  </si>
+  <si>
+    <t>284.58</t>
+  </si>
+  <si>
+    <t>89.20%</t>
+  </si>
+  <si>
+    <t>BERT_FREELB</t>
+  </si>
+  <si>
+    <t>47.30% (49.89%)</t>
+  </si>
+  <si>
+    <t>394.19</t>
+  </si>
+  <si>
+    <t>94.40%</t>
+  </si>
+  <si>
+    <t>BERT_INFOBERT</t>
+  </si>
+  <si>
+    <t>45.20% (52.07%)</t>
+  </si>
+  <si>
+    <t>373.83</t>
+  </si>
+  <si>
+    <t>94.30%</t>
+  </si>
+  <si>
+    <t>BERT_TMD</t>
+  </si>
+  <si>
+    <t>47.80% (49.04%)</t>
+  </si>
+  <si>
+    <t>833.43</t>
+  </si>
+  <si>
+    <t>93.80%</t>
+  </si>
+  <si>
+    <t>BERT_post_att_all_0.2</t>
+  </si>
+  <si>
+    <t>44.00% (52.99%)</t>
+  </si>
+  <si>
+    <t>679.69</t>
+  </si>
+  <si>
+    <t>93.60%</t>
+  </si>
+  <si>
+    <t>BERT_post_att_all_0.3</t>
+  </si>
+  <si>
+    <t>45.60% (50.97%)</t>
+  </si>
+  <si>
+    <t>738.90</t>
+  </si>
+  <si>
+    <t>93.00%</t>
+  </si>
+  <si>
+    <t>BERT_post_att_all_0.4</t>
+  </si>
+  <si>
+    <t>47.30% (49.03%)</t>
+  </si>
+  <si>
+    <t>745.41</t>
+  </si>
+  <si>
+    <t>92.80%</t>
+  </si>
+  <si>
+    <t>BERT_pre_att_all_0.2</t>
+  </si>
+  <si>
+    <t>44.80% (52.29%)</t>
+  </si>
+  <si>
+    <t>745.68</t>
+  </si>
+  <si>
+    <t>93.90%</t>
+  </si>
+  <si>
+    <t>BERT_pre_att_all_0.3</t>
+  </si>
+  <si>
+    <t>31.40% (65.76%)</t>
+  </si>
+  <si>
+    <t>630.81</t>
+  </si>
+  <si>
+    <t>91.70%</t>
+  </si>
+  <si>
+    <t>ROBERTA</t>
+  </si>
+  <si>
+    <t>38.40% (58.93%)</t>
+  </si>
+  <si>
+    <t>371.20</t>
+  </si>
+  <si>
+    <t>93.50%</t>
+  </si>
+  <si>
+    <t>ROBERTA_ASCC</t>
+  </si>
+  <si>
+    <t>49.50% (46.37%)</t>
+  </si>
+  <si>
+    <t>372.91</t>
+  </si>
+  <si>
+    <t>92.30%</t>
+  </si>
+  <si>
+    <t>ROBERTA_FREELB</t>
+  </si>
+  <si>
+    <t>50.50% (46.22%)</t>
+  </si>
+  <si>
+    <t>448.97</t>
+  </si>
+  <si>
+    <t>ROBERTA_INFOBERT</t>
+  </si>
+  <si>
+    <t>47.00% (50.11%)</t>
+  </si>
+  <si>
+    <t>394.56</t>
+  </si>
+  <si>
+    <t>ROBERTA_TMD</t>
+  </si>
+  <si>
+    <t>52.80% (43.59%)</t>
+  </si>
+  <si>
+    <t>878.22</t>
+  </si>
+  <si>
+    <t>ROBERTA_post_att_all_0.2</t>
+  </si>
+  <si>
+    <t>50.70% (45.66%)</t>
+  </si>
+  <si>
+    <t>795.98</t>
+  </si>
+  <si>
+    <t>93.30%</t>
+  </si>
+  <si>
+    <t>ROBERTA_post_att_all_0.3</t>
+  </si>
+  <si>
+    <t>50.10% (45.90%)</t>
+  </si>
+  <si>
+    <t>796.93</t>
+  </si>
+  <si>
+    <t>92.60%</t>
+  </si>
+  <si>
+    <t>ROBERTA_pre_att_all_0.2</t>
+  </si>
+  <si>
+    <t>40.80% (55.75%)</t>
+  </si>
+  <si>
+    <t>726.04</t>
+  </si>
+  <si>
+    <t>92.20%</t>
+  </si>
+  <si>
+    <t>bertattack</t>
+  </si>
+  <si>
+    <t>46.50% (50.64%)</t>
+  </si>
+  <si>
+    <t>337.84</t>
+  </si>
+  <si>
+    <t>45.90% (48.54%)</t>
+  </si>
+  <si>
+    <t>263.59</t>
+  </si>
+  <si>
+    <t>52.00% (44.92%)</t>
+  </si>
+  <si>
+    <t>370.82</t>
+  </si>
+  <si>
+    <t>56.00% (40.62%)</t>
+  </si>
+  <si>
+    <t>366.40</t>
+  </si>
+  <si>
+    <t>52.60% (43.74%)</t>
+  </si>
+  <si>
+    <t>766.72</t>
+  </si>
+  <si>
+    <t>50.30% (46.38%)</t>
+  </si>
+  <si>
+    <t>679.35</t>
+  </si>
+  <si>
+    <t>54.90% (41.35%)</t>
+  </si>
+  <si>
+    <t>727.93</t>
+  </si>
+  <si>
+    <t>54.30% (41.30%)</t>
+  </si>
+  <si>
+    <t>737.32</t>
+  </si>
+  <si>
+    <t>92.50%</t>
+  </si>
+  <si>
+    <t>53.10% (43.09%)</t>
+  </si>
+  <si>
+    <t>731.95</t>
+  </si>
+  <si>
+    <t>39.60% (56.82%)</t>
+  </si>
+  <si>
+    <t>615.00</t>
+  </si>
+  <si>
+    <t>47.30% (49.41%)</t>
+  </si>
+  <si>
+    <t>372.99</t>
+  </si>
+  <si>
+    <t>55.70% (39.65%)</t>
+  </si>
+  <si>
+    <t>374.58</t>
+  </si>
+  <si>
+    <t>58.20% (38.02%)</t>
+  </si>
+  <si>
+    <t>442.97</t>
+  </si>
+  <si>
+    <t>55.00% (41.61%)</t>
+  </si>
+  <si>
+    <t>397.35</t>
+  </si>
+  <si>
+    <t>57.90% (38.14%)</t>
+  </si>
+  <si>
+    <t>805.19</t>
+  </si>
+  <si>
+    <t>57.40% (38.74%)</t>
+  </si>
+  <si>
+    <t>772.54</t>
+  </si>
+  <si>
+    <t>93.70%</t>
+  </si>
+  <si>
+    <t>54.70% (41.06%)</t>
+  </si>
+  <si>
+    <t>740.27</t>
+  </si>
+  <si>
+    <t>46.10% (50.43%)</t>
+  </si>
+  <si>
+    <t>672.77</t>
+  </si>
+  <si>
     <t>textfooler</t>
   </si>
   <si>
-    <t>AuA(%) (ASR(%)↓)</t>
-  </si>
-  <si>
-    <t>Avg. Query↓</t>
-  </si>
-  <si>
-    <t>BERT</t>
-  </si>
-  <si>
     <t>36.80% (60.93%)</t>
   </si>
   <si>
     <t>317.27</t>
   </si>
   <si>
-    <t>94.20%</t>
-  </si>
-  <si>
-    <t>BERT_ASCC</t>
-  </si>
-  <si>
     <t>41.20% (53.81%)</t>
   </si>
   <si>
     <t>262.07</t>
   </si>
   <si>
-    <t>89.20%</t>
-  </si>
-  <si>
-    <t>BERT_FREELB</t>
-  </si>
-  <si>
     <t>49.90% (47.14%)</t>
   </si>
   <si>
     <t>356.69</t>
   </si>
   <si>
-    <t>94.40%</t>
-  </si>
-  <si>
-    <t>BERT_INFOBERT</t>
-  </si>
-  <si>
     <t>47.50% (49.63%)</t>
   </si>
   <si>
     <t>336.77</t>
   </si>
   <si>
-    <t>94.30%</t>
-  </si>
-  <si>
-    <t>BERT_TMD</t>
-  </si>
-  <si>
     <t>51.60% (44.81%)</t>
   </si>
   <si>
     <t>744.87</t>
   </si>
   <si>
-    <t>93.50%</t>
-  </si>
-  <si>
-    <t>BERT_post_att_all_0.2</t>
-  </si>
-  <si>
     <t>44.70% (52.45%)</t>
   </si>
   <si>
@@ -103,9 +397,6 @@
     <t>94.00%</t>
   </si>
   <si>
-    <t>BERT_post_att_all_0.3</t>
-  </si>
-  <si>
     <t>48.60% (48.35%)</t>
   </si>
   <si>
@@ -115,9 +406,6 @@
     <t>94.10%</t>
   </si>
   <si>
-    <t>BERT_post_att_all_0.4</t>
-  </si>
-  <si>
     <t>48.20% (48.00%)</t>
   </si>
   <si>
@@ -127,21 +415,12 @@
     <t>92.70%</t>
   </si>
   <si>
-    <t>BERT_pre_att_all_0.2</t>
-  </si>
-  <si>
     <t>49.00% (47.71%)</t>
   </si>
   <si>
     <t>675.86</t>
   </si>
   <si>
-    <t>93.70%</t>
-  </si>
-  <si>
-    <t>BERT_pre_att_all_0.3</t>
-  </si>
-  <si>
     <t>34.50% (62.34%)</t>
   </si>
   <si>
@@ -151,28 +430,28 @@
     <t>91.60%</t>
   </si>
   <si>
-    <t>ROBERTA</t>
-  </si>
-  <si>
     <t>41.00% (56.15%)</t>
   </si>
   <si>
     <t>335.88</t>
   </si>
   <si>
-    <t>ROBERTA_ASCC</t>
-  </si>
-  <si>
     <t>51.00% (44.75%)</t>
   </si>
   <si>
     <t>330.69</t>
   </si>
   <si>
-    <t>92.30%</t>
-  </si>
-  <si>
-    <t>ROBERTA_TMD</t>
+    <t>52.00% (44.62%)</t>
+  </si>
+  <si>
+    <t>402.14</t>
+  </si>
+  <si>
+    <t>48.90% (48.09%)</t>
+  </si>
+  <si>
+    <t>357.44</t>
   </si>
   <si>
     <t>55.20% (41.09%)</t>
@@ -181,33 +460,18 @@
     <t>766.74</t>
   </si>
   <si>
-    <t>ROBERTA_post_att_all_0.2</t>
-  </si>
-  <si>
     <t>49.70% (47.01%)</t>
   </si>
   <si>
     <t>683.33</t>
   </si>
   <si>
-    <t>93.80%</t>
-  </si>
-  <si>
-    <t>ROBERTA_post_att_all_0.3</t>
-  </si>
-  <si>
     <t>50.60% (45.77%)</t>
   </si>
   <si>
     <t>700.43</t>
   </si>
   <si>
-    <t>93.30%</t>
-  </si>
-  <si>
-    <t>ROBERTA_pre_att_all_0.2</t>
-  </si>
-  <si>
     <t>39.30% (57.00%)</t>
   </si>
   <si>
@@ -215,228 +479,6 @@
   </si>
   <si>
     <t>91.40%</t>
-  </si>
-  <si>
-    <t>textbugger</t>
-  </si>
-  <si>
-    <t>35.20% (62.63%)</t>
-  </si>
-  <si>
-    <t>351.92</t>
-  </si>
-  <si>
-    <t>39.30% (55.94%)</t>
-  </si>
-  <si>
-    <t>284.58</t>
-  </si>
-  <si>
-    <t>47.30% (49.89%)</t>
-  </si>
-  <si>
-    <t>394.19</t>
-  </si>
-  <si>
-    <t>45.20% (52.07%)</t>
-  </si>
-  <si>
-    <t>373.83</t>
-  </si>
-  <si>
-    <t>47.80% (49.04%)</t>
-  </si>
-  <si>
-    <t>833.43</t>
-  </si>
-  <si>
-    <t>44.00% (52.99%)</t>
-  </si>
-  <si>
-    <t>679.69</t>
-  </si>
-  <si>
-    <t>93.60%</t>
-  </si>
-  <si>
-    <t>45.60% (50.97%)</t>
-  </si>
-  <si>
-    <t>738.90</t>
-  </si>
-  <si>
-    <t>93.00%</t>
-  </si>
-  <si>
-    <t>47.30% (49.03%)</t>
-  </si>
-  <si>
-    <t>745.41</t>
-  </si>
-  <si>
-    <t>92.80%</t>
-  </si>
-  <si>
-    <t>44.80% (52.29%)</t>
-  </si>
-  <si>
-    <t>745.68</t>
-  </si>
-  <si>
-    <t>93.90%</t>
-  </si>
-  <si>
-    <t>31.40% (65.76%)</t>
-  </si>
-  <si>
-    <t>630.81</t>
-  </si>
-  <si>
-    <t>91.70%</t>
-  </si>
-  <si>
-    <t>38.40% (58.93%)</t>
-  </si>
-  <si>
-    <t>371.20</t>
-  </si>
-  <si>
-    <t>49.50% (46.37%)</t>
-  </si>
-  <si>
-    <t>372.91</t>
-  </si>
-  <si>
-    <t>52.80% (43.59%)</t>
-  </si>
-  <si>
-    <t>878.22</t>
-  </si>
-  <si>
-    <t>50.70% (45.66%)</t>
-  </si>
-  <si>
-    <t>795.98</t>
-  </si>
-  <si>
-    <t>50.10% (45.90%)</t>
-  </si>
-  <si>
-    <t>796.93</t>
-  </si>
-  <si>
-    <t>92.60%</t>
-  </si>
-  <si>
-    <t>40.80% (55.75%)</t>
-  </si>
-  <si>
-    <t>726.04</t>
-  </si>
-  <si>
-    <t>92.20%</t>
-  </si>
-  <si>
-    <t>bertattack</t>
-  </si>
-  <si>
-    <t>46.50% (50.64%)</t>
-  </si>
-  <si>
-    <t>337.84</t>
-  </si>
-  <si>
-    <t>45.90% (48.54%)</t>
-  </si>
-  <si>
-    <t>263.59</t>
-  </si>
-  <si>
-    <t>52.00% (44.92%)</t>
-  </si>
-  <si>
-    <t>370.82</t>
-  </si>
-  <si>
-    <t>56.00% (40.62%)</t>
-  </si>
-  <si>
-    <t>366.40</t>
-  </si>
-  <si>
-    <t>52.60% (43.74%)</t>
-  </si>
-  <si>
-    <t>766.72</t>
-  </si>
-  <si>
-    <t>50.30% (46.38%)</t>
-  </si>
-  <si>
-    <t>679.35</t>
-  </si>
-  <si>
-    <t>54.90% (41.35%)</t>
-  </si>
-  <si>
-    <t>727.93</t>
-  </si>
-  <si>
-    <t>54.30% (41.30%)</t>
-  </si>
-  <si>
-    <t>737.32</t>
-  </si>
-  <si>
-    <t>92.50%</t>
-  </si>
-  <si>
-    <t>53.10% (43.09%)</t>
-  </si>
-  <si>
-    <t>731.95</t>
-  </si>
-  <si>
-    <t>39.60% (56.82%)</t>
-  </si>
-  <si>
-    <t>615.00</t>
-  </si>
-  <si>
-    <t>47.30% (49.41%)</t>
-  </si>
-  <si>
-    <t>372.99</t>
-  </si>
-  <si>
-    <t>55.70% (39.65%)</t>
-  </si>
-  <si>
-    <t>374.58</t>
-  </si>
-  <si>
-    <t>57.90% (38.14%)</t>
-  </si>
-  <si>
-    <t>805.19</t>
-  </si>
-  <si>
-    <t>57.40% (38.74%)</t>
-  </si>
-  <si>
-    <t>772.54</t>
-  </si>
-  <si>
-    <t>54.70% (41.06%)</t>
-  </si>
-  <si>
-    <t>740.27</t>
-  </si>
-  <si>
-    <t>46.10% (50.43%)</t>
-  </si>
-  <si>
-    <t>672.77</t>
   </si>
 </sst>
 </file>
@@ -771,7 +813,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -799,11 +841,11 @@
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="H1" s="1"/>
     </row>
@@ -843,16 +885,16 @@
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -869,16 +911,16 @@
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -895,16 +937,16 @@
         <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -921,16 +963,16 @@
         <v>19</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -938,7 +980,7 @@
         <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>22</v>
@@ -947,16 +989,16 @@
         <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -964,7 +1006,7 @@
         <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>58</v>
+        <v>126</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>26</v>
@@ -973,16 +1015,16 @@
         <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -990,7 +1032,7 @@
         <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>80</v>
+        <v>129</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>30</v>
@@ -999,16 +1041,16 @@
         <v>31</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1016,7 +1058,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>34</v>
@@ -1025,16 +1067,16 @@
         <v>35</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1042,7 +1084,7 @@
         <v>37</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>62</v>
+        <v>108</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>38</v>
@@ -1051,16 +1093,16 @@
         <v>39</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1068,7 +1110,7 @@
         <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>92</v>
+        <v>137</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>42</v>
@@ -1077,16 +1119,16 @@
         <v>43</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1094,7 +1136,7 @@
         <v>45</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>46</v>
@@ -1103,94 +1145,94 @@
         <v>47</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="E14" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1198,7 +1240,7 @@
         <v>59</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>60</v>
@@ -1207,42 +1249,94 @@
         <v>61</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>140</v>
+      <c r="C19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>